<commit_message>
Pre Debug of the Mass for 7X7
</commit_message>
<xml_diff>
--- a/mbs-EP-v.1.0.4 - Baumgarte version/Excel Files/simple pendulum/simple_pendulum_adams.xlsx
+++ b/mbs-EP-v.1.0.4 - Baumgarte version/Excel Files/simple pendulum/simple_pendulum_adams.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.3 - changable version\Excel Files\simple pendulum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.4 - Baumgarte version\Excel Files\simple pendulum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA8E3C5-0BC5-43E5-843C-DB35CC4949F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D21379D-1087-4E1C-9968-3F8ECAD6F4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17235" yWindow="5820" windowWidth="16200" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -1290,18 +1290,66 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1311,12 +1359,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1326,46 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1386,7 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1395,7 +1398,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1407,15 +1416,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1431,6 +1431,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1464,31 +1488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1947,44 +1947,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="80"/>
-      <c r="J2" s="74" t="s">
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
+      <c r="J2" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="77"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="40">
         <v>10</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="81" t="s">
+      <c r="J3" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="81" t="s">
+      <c r="K3" s="89"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="88" t="s">
         <v>126</v>
       </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="95"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="83"/>
       <c r="P3" s="36" t="s">
         <v>156</v>
       </c>
@@ -1993,10 +1993,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="77"/>
+      <c r="C4" s="87"/>
       <c r="D4" s="40">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -2009,14 +2009,14 @@
       <c r="K4" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="84"/>
+      <c r="L4" s="98"/>
       <c r="M4" s="35" t="s">
         <v>127</v>
       </c>
       <c r="N4" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="O4" s="96"/>
+      <c r="O4" s="84"/>
       <c r="P4" s="36" t="s">
         <v>157</v>
       </c>
@@ -2025,10 +2025,10 @@
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="40" t="s">
         <v>81</v>
       </c>
@@ -2041,14 +2041,14 @@
       <c r="K5" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="84"/>
+      <c r="L5" s="98"/>
       <c r="M5" s="36" t="s">
         <v>5</v>
       </c>
       <c r="N5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="96"/>
+      <c r="O5" s="84"/>
       <c r="P5" s="36" t="s">
         <v>158</v>
       </c>
@@ -2057,10 +2057,10 @@
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="77"/>
+      <c r="C6" s="87"/>
       <c r="D6" s="40" t="s">
         <v>3</v>
       </c>
@@ -2073,14 +2073,14 @@
       <c r="K6" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="84"/>
+      <c r="L6" s="98"/>
       <c r="M6" s="36" t="s">
         <v>129</v>
       </c>
       <c r="N6" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="O6" s="96"/>
+      <c r="O6" s="84"/>
       <c r="P6" s="36" t="s">
         <v>162</v>
       </c>
@@ -2089,10 +2089,10 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="77"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="40">
         <v>-9806.65</v>
       </c>
@@ -2105,14 +2105,14 @@
       <c r="K7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="84"/>
+      <c r="L7" s="98"/>
       <c r="M7" s="36" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="96"/>
+      <c r="O7" s="84"/>
       <c r="P7" s="36" t="s">
         <v>161</v>
       </c>
@@ -2121,10 +2121,10 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="40" t="s">
         <v>235</v>
       </c>
@@ -2137,14 +2137,14 @@
       <c r="K8" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="L8" s="84"/>
+      <c r="L8" s="98"/>
       <c r="M8" s="36" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="96"/>
+      <c r="O8" s="84"/>
       <c r="P8" s="36" t="s">
         <v>165</v>
       </c>
@@ -2153,10 +2153,10 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="86" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="77"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="40"/>
       <c r="E9" s="41" t="s">
         <v>120</v>
@@ -2167,14 +2167,14 @@
       <c r="K9" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="84"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="36" t="s">
         <v>13</v>
       </c>
       <c r="N9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="96"/>
+      <c r="O9" s="84"/>
       <c r="P9" s="36" t="s">
         <v>166</v>
       </c>
@@ -2189,14 +2189,14 @@
       <c r="K10" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="84"/>
+      <c r="L10" s="98"/>
       <c r="M10" s="36" t="s">
         <v>14</v>
       </c>
       <c r="N10" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="96"/>
+      <c r="O10" s="84"/>
       <c r="P10" s="39" t="s">
         <v>167</v>
       </c>
@@ -2207,14 +2207,14 @@
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="J11" s="43"/>
       <c r="K11" s="44"/>
-      <c r="L11" s="84"/>
+      <c r="L11" s="98"/>
       <c r="M11" s="36" t="s">
         <v>131</v>
       </c>
       <c r="N11" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="96"/>
+      <c r="O11" s="84"/>
       <c r="P11" s="39" t="s">
         <v>168</v>
       </c>
@@ -2223,25 +2223,25 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
       <c r="J12" s="45"/>
       <c r="K12" s="46"/>
-      <c r="L12" s="84"/>
+      <c r="L12" s="98"/>
       <c r="M12" s="36" t="s">
         <v>132</v>
       </c>
       <c r="N12" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="O12" s="96"/>
+      <c r="O12" s="84"/>
       <c r="P12" s="36" t="s">
         <v>173</v>
       </c>
@@ -2250,29 +2250,29 @@
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="75"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="55" t="s">
         <v>234</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F13" s="99"/>
-      <c r="G13" s="99"/>
-      <c r="H13" s="99"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
       <c r="J13" s="45"/>
       <c r="K13" s="46"/>
-      <c r="L13" s="84"/>
+      <c r="L13" s="98"/>
       <c r="M13" s="36" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="96"/>
+      <c r="O13" s="84"/>
       <c r="P13" s="39" t="s">
         <v>174</v>
       </c>
@@ -2281,29 +2281,29 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="75"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="55" t="s">
         <v>234</v>
       </c>
       <c r="E14" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
       <c r="J14" s="47"/>
       <c r="K14" s="48"/>
-      <c r="L14" s="84"/>
+      <c r="L14" s="98"/>
       <c r="M14" s="36" t="s">
         <v>133</v>
       </c>
       <c r="N14" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="O14" s="96"/>
+      <c r="O14" s="84"/>
       <c r="P14" s="39" t="s">
         <v>175</v>
       </c>
@@ -2312,31 +2312,31 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="75"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="68" t="s">
         <v>234</v>
       </c>
       <c r="E15" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="J15" s="81" t="s">
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="J15" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="K15" s="82"/>
-      <c r="L15" s="84"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="98"/>
       <c r="M15" s="36" t="s">
         <v>15</v>
       </c>
       <c r="N15" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="96"/>
+      <c r="O15" s="84"/>
       <c r="P15" s="39" t="s">
         <v>176</v>
       </c>
@@ -2345,33 +2345,33 @@
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="75"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="68" t="s">
         <v>234</v>
       </c>
       <c r="E16" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
       <c r="J16" s="36" t="s">
         <v>93</v>
       </c>
       <c r="K16" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="L16" s="84"/>
+      <c r="L16" s="98"/>
       <c r="M16" s="36" t="s">
         <v>134</v>
       </c>
       <c r="N16" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="O16" s="96"/>
+      <c r="O16" s="84"/>
       <c r="P16" s="36" t="s">
         <v>181</v>
       </c>
@@ -2380,31 +2380,31 @@
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="75"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="68" t="s">
         <v>234</v>
       </c>
       <c r="E17" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F17" s="99"/>
-      <c r="G17" s="99"/>
-      <c r="H17" s="99"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
       <c r="J17" s="36" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="L17" s="84"/>
-      <c r="M17" s="81" t="s">
+      <c r="L17" s="98"/>
+      <c r="M17" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="N17" s="82"/>
-      <c r="O17" s="96"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="84"/>
       <c r="P17" s="39" t="s">
         <v>182</v>
       </c>
@@ -2413,33 +2413,33 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="85" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="75"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="68" t="s">
         <v>234</v>
       </c>
       <c r="E18" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
       <c r="J18" s="36" t="s">
         <v>94</v>
       </c>
       <c r="K18" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="L18" s="84"/>
+      <c r="L18" s="98"/>
       <c r="M18" s="42" t="s">
         <v>155</v>
       </c>
       <c r="N18" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="O18" s="96"/>
+      <c r="O18" s="84"/>
       <c r="P18" s="39" t="s">
         <v>183</v>
       </c>
@@ -2448,31 +2448,31 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="75"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="55"/>
       <c r="E19" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
       <c r="J19" s="36" t="s">
         <v>95</v>
       </c>
       <c r="K19" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="84"/>
+      <c r="L19" s="98"/>
       <c r="M19" s="37" t="s">
         <v>147</v>
       </c>
       <c r="N19" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="O19" s="96"/>
+      <c r="O19" s="84"/>
       <c r="P19" s="39" t="s">
         <v>184</v>
       </c>
@@ -2481,33 +2481,33 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="C20" s="75"/>
+      <c r="C20" s="85"/>
       <c r="D20" s="55" t="s">
         <v>234</v>
       </c>
       <c r="E20" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
       <c r="J20" s="36" t="s">
         <v>101</v>
       </c>
       <c r="K20" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="L20" s="84"/>
+      <c r="L20" s="98"/>
       <c r="M20" s="37" t="s">
         <v>148</v>
       </c>
       <c r="N20" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="O20" s="96"/>
+      <c r="O20" s="84"/>
       <c r="P20" s="36" t="s">
         <v>189</v>
       </c>
@@ -2516,31 +2516,31 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="85" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="75"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="99"/>
-      <c r="G21" s="99"/>
-      <c r="H21" s="99"/>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
       <c r="J21" s="36" t="s">
         <v>96</v>
       </c>
       <c r="K21" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="84"/>
+      <c r="L21" s="98"/>
       <c r="M21" s="37" t="s">
         <v>149</v>
       </c>
       <c r="N21" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="O21" s="96"/>
+      <c r="O21" s="84"/>
       <c r="P21" s="39" t="s">
         <v>190</v>
       </c>
@@ -2549,20 +2549,20 @@
       </c>
     </row>
     <row r="22" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="97"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="55">
         <v>3</v>
       </c>
-      <c r="E22" s="98" t="s">
+      <c r="E22" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="F22" s="98" t="s">
+      <c r="F22" s="91" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="98"/>
+      <c r="G22" s="91"/>
       <c r="H22" s="56"/>
       <c r="J22" s="26" t="s">
         <v>107</v>
@@ -2570,14 +2570,14 @@
       <c r="K22" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="L22" s="85"/>
+      <c r="L22" s="99"/>
       <c r="M22" s="37" t="s">
         <v>150</v>
       </c>
       <c r="N22" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="O22" s="96"/>
+      <c r="O22" s="84"/>
       <c r="P22" s="39" t="s">
         <v>191</v>
       </c>
@@ -2586,19 +2586,19 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="55"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
       <c r="H23" s="56"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="96"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="76"/>
+      <c r="O23" s="84"/>
       <c r="P23" s="39" t="s">
         <v>192</v>
       </c>
@@ -2607,19 +2607,19 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
       <c r="D24" s="55"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="91"/>
       <c r="H24" s="56"/>
-      <c r="J24" s="89"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="96"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="84"/>
       <c r="P24" s="26" t="s">
         <v>198</v>
       </c>
@@ -2628,19 +2628,19 @@
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="55"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="91"/>
       <c r="H25" s="56"/>
-      <c r="J25" s="89"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="96"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="84"/>
       <c r="P25" s="26" t="s">
         <v>202</v>
       </c>
@@ -2649,19 +2649,19 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="97"/>
-      <c r="C26" s="97"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
       <c r="H26" s="56"/>
-      <c r="J26" s="89"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="90"/>
-      <c r="N26" s="91"/>
-      <c r="O26" s="96"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="84"/>
       <c r="P26" s="26" t="s">
         <v>203</v>
       </c>
@@ -2670,19 +2670,19 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
       <c r="H27" s="56"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="96"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="84"/>
       <c r="P27" s="26" t="s">
         <v>204</v>
       </c>
@@ -2691,19 +2691,19 @@
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="98"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
       <c r="H28" s="56"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="96"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="84"/>
       <c r="P28" s="26" t="s">
         <v>206</v>
       </c>
@@ -2712,19 +2712,19 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="98"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
       <c r="H29" s="56"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="91"/>
-      <c r="O29" s="96"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="84"/>
       <c r="P29" s="26" t="s">
         <v>205</v>
       </c>
@@ -2733,12 +2733,12 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J30" s="89"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="91"/>
-      <c r="O30" s="96"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="84"/>
       <c r="P30" s="26" t="s">
         <v>207</v>
       </c>
@@ -2747,12 +2747,12 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J31" s="89"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="90"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="96"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="84"/>
       <c r="P31" s="26" t="s">
         <v>208</v>
       </c>
@@ -2761,12 +2761,12 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J32" s="89"/>
-      <c r="K32" s="90"/>
-      <c r="L32" s="90"/>
-      <c r="M32" s="90"/>
-      <c r="N32" s="91"/>
-      <c r="O32" s="96"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="84"/>
       <c r="P32" s="26" t="s">
         <v>209</v>
       </c>
@@ -2775,12 +2775,12 @@
       </c>
     </row>
     <row r="33" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J33" s="89"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="91"/>
-      <c r="O33" s="96"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="84"/>
       <c r="P33" s="26" t="s">
         <v>210</v>
       </c>
@@ -2789,12 +2789,12 @@
       </c>
     </row>
     <row r="34" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J34" s="89"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="91"/>
-      <c r="O34" s="96"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="84"/>
       <c r="P34" s="26" t="s">
         <v>211</v>
       </c>
@@ -2803,12 +2803,12 @@
       </c>
     </row>
     <row r="35" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J35" s="89"/>
-      <c r="K35" s="90"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="91"/>
-      <c r="O35" s="96"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="84"/>
       <c r="P35" s="26" t="s">
         <v>212</v>
       </c>
@@ -2817,12 +2817,12 @@
       </c>
     </row>
     <row r="36" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J36" s="89"/>
-      <c r="K36" s="90"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="90"/>
-      <c r="N36" s="91"/>
-      <c r="O36" s="96"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="79"/>
+      <c r="O36" s="84"/>
       <c r="P36" s="26" t="s">
         <v>221</v>
       </c>
@@ -2831,12 +2831,12 @@
       </c>
     </row>
     <row r="37" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J37" s="89"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="90"/>
-      <c r="M37" s="90"/>
-      <c r="N37" s="91"/>
-      <c r="O37" s="96"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="84"/>
       <c r="P37" s="26" t="s">
         <v>222</v>
       </c>
@@ -2845,12 +2845,12 @@
       </c>
     </row>
     <row r="38" spans="10:17" x14ac:dyDescent="0.25">
-      <c r="J38" s="92"/>
-      <c r="K38" s="93"/>
-      <c r="L38" s="93"/>
-      <c r="M38" s="93"/>
-      <c r="N38" s="94"/>
-      <c r="O38" s="96"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="81"/>
+      <c r="L38" s="81"/>
+      <c r="M38" s="81"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="84"/>
       <c r="P38" s="26" t="s">
         <v>223</v>
       </c>
@@ -2868,6 +2868,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:L22"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="J23:N38"/>
     <mergeCell ref="O3:O38"/>
     <mergeCell ref="B18:C18"/>
@@ -2883,21 +2898,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="F13:H21"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:L22"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2910,7 +2910,7 @@
   <dimension ref="A1:AK194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2929,32 +2929,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="99"/>
-      <c r="B1" s="99"/>
-      <c r="C1" s="75" t="s">
+      <c r="A1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75" t="s">
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75" t="s">
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75" t="s">
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
       <c r="S1" s="52" t="s">
         <v>34</v>
       </c>
@@ -2978,69 +2978,69 @@
       <c r="AK1" s="52"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="106" t="s">
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106" t="s">
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106" t="s">
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="75" t="s">
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75" t="s">
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="98" t="s">
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="91" t="s">
         <v>83</v>
       </c>
       <c r="S2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="103" t="s">
+      <c r="T2" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="U2" s="104"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="100" t="s">
+      <c r="U2" s="105"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="102"/>
-      <c r="Z2" s="100" t="s">
+      <c r="X2" s="102"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="101" t="s">
         <v>90</v>
       </c>
-      <c r="AA2" s="101"/>
-      <c r="AB2" s="102"/>
-      <c r="AC2" s="100" t="s">
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="103"/>
+      <c r="AC2" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="101"/>
-      <c r="AE2" s="102"/>
-      <c r="AF2" s="100" t="s">
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="AG2" s="101"/>
-      <c r="AH2" s="102"/>
-      <c r="AI2" s="100" t="s">
+      <c r="AG2" s="102"/>
+      <c r="AH2" s="103"/>
+      <c r="AI2" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="AJ2" s="101"/>
-      <c r="AK2" s="102"/>
+      <c r="AJ2" s="102"/>
+      <c r="AK2" s="103"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -3094,7 +3094,7 @@
       <c r="Q3" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="98"/>
+      <c r="R3" s="91"/>
       <c r="S3" s="53"/>
       <c r="T3" s="54" t="s">
         <v>61</v>
@@ -3207,16 +3207,16 @@
         <v>0</v>
       </c>
       <c r="S4" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="52">
         <v>0</v>
@@ -6528,6 +6528,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="O2:Q2"/>
@@ -6539,12 +6545,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6575,16 +6575,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -6615,11 +6615,11 @@
       <c r="E2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -6675,19 +6675,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -6712,16 +6712,16 @@
       <c r="E6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="110" t="s">
+      <c r="F6" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="111"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="110" t="s">
+      <c r="G6" s="114"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="111"/>
-      <c r="K6" s="112"/>
+      <c r="J6" s="114"/>
+      <c r="K6" s="115"/>
       <c r="L6" s="19"/>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
@@ -6757,22 +6757,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="107"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -6797,21 +6797,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="108" t="s">
+      <c r="F9" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="109" t="s">
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
-      <c r="L9" s="109" t="s">
+      <c r="J9" s="107"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="107" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="107"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -6842,19 +6842,19 @@
       <c r="X10" s="10"/>
     </row>
     <row r="11" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="107"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="107"/>
-      <c r="K11" s="107"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="108"/>
+      <c r="J11" s="108"/>
+      <c r="K11" s="108"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -6879,16 +6879,16 @@
       <c r="E12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="108" t="s">
+      <c r="F12" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="109" t="s">
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="109"/>
-      <c r="K12" s="109"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -6990,19 +6990,19 @@
       <c r="X15" s="10"/>
     </row>
     <row r="16" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="107" t="s">
+      <c r="A16" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="107"/>
-      <c r="C16" s="107"/>
-      <c r="D16" s="107"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="K16" s="107"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="108"/>
+      <c r="K16" s="108"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
@@ -7027,16 +7027,16 @@
       <c r="E17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="108" t="s">
+      <c r="F17" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="109" t="s">
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="107"/>
     </row>
     <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
@@ -7073,19 +7073,19 @@
       <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="107" t="s">
+      <c r="A20" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="107"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
@@ -7110,36 +7110,36 @@
       <c r="E21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="108" t="s">
+      <c r="F21" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="109" t="s">
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
     </row>
     <row r="22" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:24" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="108" t="s">
         <v>121</v>
       </c>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="107"/>
-      <c r="K24" s="107"/>
-      <c r="L24" s="107"/>
-      <c r="M24" s="107"/>
-      <c r="N24" s="107"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="108"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="108"/>
+      <c r="I24" s="108"/>
+      <c r="J24" s="108"/>
+      <c r="K24" s="108"/>
+      <c r="L24" s="108"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="108"/>
     </row>
     <row r="25" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -7157,44 +7157,44 @@
       <c r="E25" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="108" t="s">
+      <c r="F25" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="109" t="s">
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109" t="s">
+      <c r="J25" s="107"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="107" t="s">
         <v>122</v>
       </c>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="107"/>
     </row>
     <row r="26" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:24" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="108" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="108"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="108"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="108"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="108"/>
     </row>
     <row r="29" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
@@ -7212,26 +7212,26 @@
       <c r="E29" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="110" t="s">
+      <c r="F29" s="113" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="111"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="110" t="s">
+      <c r="G29" s="114"/>
+      <c r="H29" s="115"/>
+      <c r="I29" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="J29" s="111"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="109" t="s">
+      <c r="J29" s="114"/>
+      <c r="K29" s="115"/>
+      <c r="L29" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109" t="s">
+      <c r="M29" s="107"/>
+      <c r="N29" s="107"/>
+      <c r="O29" s="107" t="s">
         <v>125</v>
       </c>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="109"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
     </row>
     <row r="30" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
@@ -7254,14 +7254,14 @@
     </row>
     <row r="31" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="107" t="s">
+      <c r="A32" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="107"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="107"/>
-      <c r="F32" s="107"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -7335,12 +7335,12 @@
       <c r="X35" s="10"/>
     </row>
     <row r="36" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="107" t="s">
+      <c r="A36" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="107"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -7412,15 +7412,15 @@
       <c r="K39" s="11"/>
     </row>
     <row r="40" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="113" t="s">
+      <c r="A40" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="114"/>
-      <c r="C40" s="114"/>
-      <c r="D40" s="114"/>
-      <c r="E40" s="114"/>
-      <c r="F40" s="114"/>
-      <c r="G40" s="115"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="112"/>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
@@ -7440,11 +7440,11 @@
       <c r="D41" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="109" t="s">
+      <c r="E41" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="F41" s="109"/>
-      <c r="G41" s="109"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="107"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="10"/>
@@ -7512,6 +7512,21 @@
     <row r="60" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:K17"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="A20:K20"/>
     <mergeCell ref="F21:H21"/>
@@ -7528,21 +7543,6 @@
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="L29:N29"/>
     <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -7611,11 +7611,11 @@
       <c r="E2" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="109" t="s">
+      <c r="F2" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
       <c r="I2" s="60" t="s">
         <v>239</v>
       </c>
@@ -7715,19 +7715,19 @@
       <c r="S1" s="117"/>
     </row>
     <row r="2" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
+      <c r="A2" s="108"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
       <c r="N2" s="118" t="s">
         <v>242</v>
       </c>
@@ -7736,14 +7736,14 @@
       <c r="Q2" s="119"/>
       <c r="R2" s="119"/>
       <c r="S2" s="120"/>
-      <c r="AB2" s="121" t="s">
+      <c r="AB2" s="129" t="s">
         <v>118</v>
       </c>
-      <c r="AC2" s="122"/>
-      <c r="AD2" s="122"/>
-      <c r="AE2" s="122"/>
-      <c r="AF2" s="122"/>
-      <c r="AG2" s="123"/>
+      <c r="AC2" s="130"/>
+      <c r="AD2" s="130"/>
+      <c r="AE2" s="130"/>
+      <c r="AF2" s="130"/>
+      <c r="AG2" s="131"/>
     </row>
     <row r="3" spans="1:33" s="28" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
@@ -7761,16 +7761,16 @@
       <c r="E3" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="133"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="135" t="s">
+      <c r="G3" s="140"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="128"/>
       <c r="L3" s="62" t="s">
         <v>243</v>
       </c>
@@ -7789,16 +7789,16 @@
       <c r="Q3" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="130" t="s">
+      <c r="R3" s="138" t="s">
         <v>117</v>
       </c>
-      <c r="S3" s="130"/>
-      <c r="AB3" s="124"/>
-      <c r="AC3" s="125"/>
-      <c r="AD3" s="125"/>
-      <c r="AE3" s="125"/>
-      <c r="AF3" s="125"/>
-      <c r="AG3" s="126"/>
+      <c r="S3" s="138"/>
+      <c r="AB3" s="132"/>
+      <c r="AC3" s="133"/>
+      <c r="AD3" s="133"/>
+      <c r="AE3" s="133"/>
+      <c r="AF3" s="133"/>
+      <c r="AG3" s="134"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
@@ -7818,12 +7818,12 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
-      <c r="AB4" s="124"/>
-      <c r="AC4" s="125"/>
-      <c r="AD4" s="125"/>
-      <c r="AE4" s="125"/>
-      <c r="AF4" s="125"/>
-      <c r="AG4" s="126"/>
+      <c r="AB4" s="132"/>
+      <c r="AC4" s="133"/>
+      <c r="AD4" s="133"/>
+      <c r="AE4" s="133"/>
+      <c r="AF4" s="133"/>
+      <c r="AG4" s="134"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
@@ -7845,20 +7845,20 @@
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
       <c r="S5" s="38"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="125"/>
-      <c r="AD5" s="125"/>
-      <c r="AE5" s="125"/>
-      <c r="AF5" s="125"/>
-      <c r="AG5" s="126"/>
+      <c r="AB5" s="132"/>
+      <c r="AC5" s="133"/>
+      <c r="AD5" s="133"/>
+      <c r="AE5" s="133"/>
+      <c r="AF5" s="133"/>
+      <c r="AG5" s="134"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AB6" s="124"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="125"/>
-      <c r="AE6" s="125"/>
-      <c r="AF6" s="125"/>
-      <c r="AG6" s="126"/>
+      <c r="AB6" s="132"/>
+      <c r="AC6" s="133"/>
+      <c r="AD6" s="133"/>
+      <c r="AE6" s="133"/>
+      <c r="AF6" s="133"/>
+      <c r="AG6" s="134"/>
     </row>
     <row r="7" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="116" t="s">
@@ -7881,40 +7881,40 @@
       <c r="P7" s="117"/>
       <c r="Q7" s="117"/>
       <c r="R7" s="117"/>
-      <c r="AB7" s="124"/>
-      <c r="AC7" s="125"/>
-      <c r="AD7" s="125"/>
-      <c r="AE7" s="125"/>
-      <c r="AF7" s="125"/>
-      <c r="AG7" s="126"/>
+      <c r="AB7" s="132"/>
+      <c r="AC7" s="133"/>
+      <c r="AD7" s="133"/>
+      <c r="AE7" s="133"/>
+      <c r="AF7" s="133"/>
+      <c r="AG7" s="134"/>
     </row>
     <row r="8" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="107"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107"/>
-      <c r="J8" s="107"/>
-      <c r="K8" s="107"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="131" t="s">
+      <c r="A8" s="108"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="139" t="s">
         <v>244</v>
       </c>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131"/>
-      <c r="AB8" s="124"/>
-      <c r="AC8" s="125"/>
-      <c r="AD8" s="125"/>
-      <c r="AE8" s="125"/>
-      <c r="AF8" s="125"/>
-      <c r="AG8" s="126"/>
+      <c r="O8" s="139"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="139"/>
+      <c r="AB8" s="132"/>
+      <c r="AC8" s="133"/>
+      <c r="AD8" s="133"/>
+      <c r="AE8" s="133"/>
+      <c r="AF8" s="133"/>
+      <c r="AG8" s="134"/>
     </row>
     <row r="9" spans="1:33" s="28" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
@@ -7932,16 +7932,16 @@
       <c r="E9" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="132" t="s">
+      <c r="F9" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="133"/>
-      <c r="H9" s="134"/>
-      <c r="I9" s="135" t="s">
+      <c r="G9" s="140"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="136"/>
-      <c r="K9" s="137"/>
+      <c r="J9" s="127"/>
+      <c r="K9" s="128"/>
       <c r="L9" s="31" t="s">
         <v>111</v>
       </c>
@@ -7957,16 +7957,16 @@
       <c r="P9" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="Q9" s="132" t="s">
+      <c r="Q9" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="R9" s="134"/>
-      <c r="AB9" s="124"/>
-      <c r="AC9" s="125"/>
-      <c r="AD9" s="125"/>
-      <c r="AE9" s="125"/>
-      <c r="AF9" s="125"/>
-      <c r="AG9" s="126"/>
+      <c r="R9" s="125"/>
+      <c r="AB9" s="132"/>
+      <c r="AC9" s="133"/>
+      <c r="AD9" s="133"/>
+      <c r="AE9" s="133"/>
+      <c r="AF9" s="133"/>
+      <c r="AG9" s="134"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="38"/>
@@ -7982,12 +7982,12 @@
       <c r="K10" s="38"/>
       <c r="L10" s="64"/>
       <c r="M10" s="23"/>
-      <c r="AB10" s="124"/>
-      <c r="AC10" s="125"/>
-      <c r="AD10" s="125"/>
-      <c r="AE10" s="125"/>
-      <c r="AF10" s="125"/>
-      <c r="AG10" s="126"/>
+      <c r="AB10" s="132"/>
+      <c r="AC10" s="133"/>
+      <c r="AD10" s="133"/>
+      <c r="AE10" s="133"/>
+      <c r="AF10" s="133"/>
+      <c r="AG10" s="134"/>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="38"/>
@@ -8002,21 +8002,21 @@
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
       <c r="L11" s="64"/>
-      <c r="AB11" s="124"/>
-      <c r="AC11" s="125"/>
-      <c r="AD11" s="125"/>
-      <c r="AE11" s="125"/>
-      <c r="AF11" s="125"/>
-      <c r="AG11" s="126"/>
+      <c r="AB11" s="132"/>
+      <c r="AC11" s="133"/>
+      <c r="AD11" s="133"/>
+      <c r="AE11" s="133"/>
+      <c r="AF11" s="133"/>
+      <c r="AG11" s="134"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Q12" s="38"/>
-      <c r="AB12" s="124"/>
-      <c r="AC12" s="125"/>
-      <c r="AD12" s="125"/>
-      <c r="AE12" s="125"/>
-      <c r="AF12" s="125"/>
-      <c r="AG12" s="126"/>
+      <c r="AB12" s="132"/>
+      <c r="AC12" s="133"/>
+      <c r="AD12" s="133"/>
+      <c r="AE12" s="133"/>
+      <c r="AF12" s="133"/>
+      <c r="AG12" s="134"/>
     </row>
     <row r="13" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="116" t="s">
@@ -8046,33 +8046,33 @@
       <c r="W13" s="117"/>
       <c r="X13" s="117"/>
       <c r="Y13" s="117"/>
-      <c r="AB13" s="127"/>
-      <c r="AC13" s="128"/>
-      <c r="AD13" s="128"/>
-      <c r="AE13" s="128"/>
-      <c r="AF13" s="128"/>
-      <c r="AG13" s="129"/>
+      <c r="AB13" s="135"/>
+      <c r="AC13" s="136"/>
+      <c r="AD13" s="136"/>
+      <c r="AE13" s="136"/>
+      <c r="AF13" s="136"/>
+      <c r="AG13" s="137"/>
     </row>
     <row r="14" spans="1:33" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="114"/>
-      <c r="H14" s="114"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="114"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="114"/>
-      <c r="O14" s="114"/>
-      <c r="P14" s="114"/>
-      <c r="Q14" s="114"/>
-      <c r="R14" s="114"/>
-      <c r="S14" s="115"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
+      <c r="R14" s="111"/>
+      <c r="S14" s="112"/>
       <c r="T14" s="118" t="s">
         <v>245</v>
       </c>
@@ -8100,26 +8100,26 @@
       <c r="E15" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="97" t="s">
+      <c r="F15" s="90" t="s">
         <v>246</v>
       </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="135" t="s">
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="126" t="s">
         <v>247</v>
       </c>
-      <c r="J15" s="136"/>
-      <c r="K15" s="137"/>
-      <c r="L15" s="138" t="s">
+      <c r="J15" s="127"/>
+      <c r="K15" s="128"/>
+      <c r="L15" s="121" t="s">
         <v>248</v>
       </c>
-      <c r="M15" s="139"/>
-      <c r="N15" s="140"/>
-      <c r="O15" s="138" t="s">
+      <c r="M15" s="122"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="121" t="s">
         <v>249</v>
       </c>
-      <c r="P15" s="139"/>
-      <c r="Q15" s="140"/>
+      <c r="P15" s="122"/>
+      <c r="Q15" s="123"/>
       <c r="R15" s="31" t="s">
         <v>73</v>
       </c>
@@ -8138,10 +8138,10 @@
       <c r="W15" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="X15" s="132" t="s">
+      <c r="X15" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="Y15" s="134"/>
+      <c r="Y15" s="125"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
@@ -8245,16 +8245,16 @@
       <c r="E20" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="97" t="s">
+      <c r="F20" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="138" t="s">
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="121" t="s">
         <v>154</v>
       </c>
-      <c r="J20" s="139"/>
-      <c r="K20" s="140"/>
+      <c r="J20" s="122"/>
+      <c r="K20" s="123"/>
       <c r="L20" s="61" t="s">
         <v>112</v>
       </c>
@@ -8267,10 +8267,10 @@
       <c r="O20" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="P20" s="132" t="s">
+      <c r="P20" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="Q20" s="134"/>
+      <c r="Q20" s="125"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
@@ -8319,16 +8319,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="L19:Q19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="T14:Y14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="X15:Y15"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A14:S14"/>
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:S2"/>
     <mergeCell ref="AB2:AG13"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="A8:M8"/>
@@ -8340,11 +8335,16 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A14:S14"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="L19:Q19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="T14:Y14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="X15:Y15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8367,21 +8367,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="108" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="F1" s="78" t="s">
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="F1" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="80"/>
-      <c r="I1" s="78" t="s">
+      <c r="G1" s="96"/>
+      <c r="I1" s="94" t="s">
         <v>233</v>
       </c>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="80"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="96"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">

</xml_diff>